<commit_message>
Filters Left first test
</commit_message>
<xml_diff>
--- a/management/TASK.xlsx
+++ b/management/TASK.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
   <si>
     <t>%</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>24-dec - 27 dec</t>
+  </si>
+  <si>
+    <t>https://docs.mongodb.org/v3.0/reference/operator/aggregation/sum/</t>
+  </si>
+  <si>
+    <t>Operations Sum</t>
+  </si>
+  <si>
+    <t>24-dec - 29 dec</t>
+  </si>
+  <si>
+    <t>26-dec - 27 dec</t>
   </si>
 </sst>
 </file>
@@ -296,7 +308,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="118">
+  <cellStyleXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -415,8 +427,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -434,8 +462,9 @@
     <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="128"/>
   </cellXfs>
-  <cellStyles count="118">
+  <cellStyles count="134">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -494,6 +523,16 @@
     <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -552,6 +591,12 @@
     <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -884,16 +929,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="13"/>
     <col min="6" max="6" width="36.1640625" style="13" customWidth="1"/>
     <col min="7" max="7" width="30.33203125" customWidth="1"/>
@@ -939,12 +984,18 @@
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
@@ -986,7 +1037,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="6"/>
@@ -1268,7 +1319,9 @@
       <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="6"/>
+      <c r="A31" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="B31" s="6" t="s">
         <v>15</v>
       </c>
@@ -1364,15 +1417,21 @@
       <c r="G36" s="6"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="15">
         <v>0</v>
       </c>
       <c r="F37" s="15"/>
-      <c r="G37" s="6"/>
+      <c r="G37" s="17" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="6"/>
@@ -1838,6 +1897,9 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="G37" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>